<commit_message>
adding Iqaluit weather files. Updated btap/Weatherdata to include moncton and iqaluit
</commit_message>
<xml_diff>
--- a/lib/openstudio-standards/btap/WeatherData1.xlsx
+++ b/lib/openstudio-standards/btap/WeatherData1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymahone\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Files\Devel\OpenStudio-Standards\openstudio-standards\lib\openstudio-standards\btap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="376">
   <si>
     <t>file</t>
   </si>
@@ -1132,12 +1132,30 @@
   </si>
   <si>
     <t>CAN_PQ_Bagotville.717270_CWEC.epw'</t>
+  </si>
+  <si>
+    <t>CAN_NU_Iqaluit.AP.719090_CWEC2016.epw</t>
+  </si>
+  <si>
+    <t>Iqaluit AP_NU_CAN</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>Iqaluit</t>
+  </si>
+  <si>
+    <t>FuelOilNo2</t>
+  </si>
+  <si>
+    <t>CAN_NU_Iqaluit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1506,10 +1524,10 @@
   <dimension ref="A1:Y82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
+      <selection pane="bottomRight" activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7654,7 +7672,81 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>370</v>
+      </c>
+      <c r="B81" t="s">
+        <v>375</v>
+      </c>
+      <c r="C81" t="s">
+        <v>371</v>
+      </c>
+      <c r="D81" t="s">
+        <v>59</v>
+      </c>
+      <c r="E81" t="s">
+        <v>372</v>
+      </c>
+      <c r="F81" t="s">
+        <v>373</v>
+      </c>
+      <c r="G81">
+        <v>9794</v>
+      </c>
+      <c r="I81">
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>63.75</v>
+      </c>
+      <c r="K81">
+        <v>-68.55</v>
+      </c>
+      <c r="L81">
+        <v>34</v>
+      </c>
+      <c r="M81">
+        <v>11</v>
+      </c>
+      <c r="N81" s="3">
+        <v>8</v>
+      </c>
+      <c r="O81" t="s">
+        <v>374</v>
+      </c>
+      <c r="P81" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q81" t="s">
+        <v>100</v>
+      </c>
+      <c r="R81" t="s">
+        <v>98</v>
+      </c>
+      <c r="S81" t="s">
+        <v>103</v>
+      </c>
+      <c r="T81" t="s">
+        <v>105</v>
+      </c>
+      <c r="U81" t="s">
+        <v>97</v>
+      </c>
+      <c r="V81" t="s">
+        <v>97</v>
+      </c>
+      <c r="W81" t="s">
+        <v>97</v>
+      </c>
+      <c r="X81" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="H82" s="6"/>
     </row>
   </sheetData>

</xml_diff>